<commit_message>
Corrected error in s_profile
</commit_message>
<xml_diff>
--- a/source_environmental_conditions.xlsx
+++ b/source_environmental_conditions.xlsx
@@ -85,7 +85,7 @@
     <t xml:space="preserve">stratification_type</t>
   </si>
   <si>
-    <t xml:space="preserve">step</t>
+    <t xml:space="preserve">uniform</t>
   </si>
   <si>
     <t xml:space="preserve">step_height</t>
@@ -415,7 +415,7 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -484,7 +484,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>1.05</v>
+        <v>0.998</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -492,7 +492,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>1.01</v>
+        <v>0.998</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Updated documentation, and edits to README.md
</commit_message>
<xml_diff>
--- a/source_environmental_conditions.xlsx
+++ b/source_environmental_conditions.xlsx
@@ -85,7 +85,7 @@
     <t xml:space="preserve">stratification_type</t>
   </si>
   <si>
-    <t xml:space="preserve">uniform</t>
+    <t xml:space="preserve">step</t>
   </si>
   <si>
     <t xml:space="preserve">step_height</t>
@@ -415,7 +415,7 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>